<commit_message>
Atualiza relatório final e adiciona versão em PDF
</commit_message>
<xml_diff>
--- a/Medicoes/tabela_tempos.xlsx
+++ b/Medicoes/tabela_tempos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DELL\Desktop\ASD 5° Semestre\OBJETOS INTELIGENTES CONECTADOS\AULA 04\Projeto-Monitoramento-ESP32\Medicoes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E816E176-7D85-435B-9325-2C66F706BDE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{416BE621-7F6B-4199-9BFA-D10FD997BD19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{E6E2EC0F-87DA-4E3D-B494-5A592BE21A1C}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
   <si>
     <t>Data</t>
   </si>
@@ -57,6 +57,24 @@
   </si>
   <si>
     <t>26.1</t>
+  </si>
+  <si>
+    <t>Nível de Água (cm)</t>
+  </si>
+  <si>
+    <t>24.6</t>
+  </si>
+  <si>
+    <t>25.1</t>
+  </si>
+  <si>
+    <t>25.6</t>
+  </si>
+  <si>
+    <t>24.0</t>
+  </si>
+  <si>
+    <t>25.4</t>
   </si>
 </sst>
 </file>
@@ -115,7 +133,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -130,6 +148,15 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -464,10 +491,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5958E279-C96B-4444-81CD-687001D4E006}">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -480,7 +507,7 @@
     <col min="6" max="6" width="23.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -496,8 +523,11 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>45803</v>
       </c>
@@ -513,8 +543,11 @@
       <c r="E2" s="4">
         <v>120</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F2" s="6">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>45803</v>
       </c>
@@ -530,55 +563,137 @@
       <c r="E3" s="4">
         <v>115</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="5"/>
-      <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="5"/>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="5"/>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="5"/>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="5"/>
-      <c r="B8" s="5"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="5"/>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F3" s="6">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>45803</v>
+      </c>
+      <c r="B4" s="7">
+        <v>0.59375</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="6">
+        <v>59</v>
+      </c>
+      <c r="E4" s="6">
+        <v>114</v>
+      </c>
+      <c r="F4" s="6">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
+        <v>45803</v>
+      </c>
+      <c r="B5" s="7">
+        <v>0.59722222222222221</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="6">
+        <v>52</v>
+      </c>
+      <c r="E5" s="6">
+        <v>120</v>
+      </c>
+      <c r="F5" s="6">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="8">
+        <v>45803</v>
+      </c>
+      <c r="B6" s="7">
+        <v>0.61111111111111116</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="6">
+        <v>48</v>
+      </c>
+      <c r="E6" s="6">
+        <v>115</v>
+      </c>
+      <c r="F6" s="6">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="8">
+        <v>45803</v>
+      </c>
+      <c r="B7" s="7">
+        <v>0.62013888888888891</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="6">
+        <v>54</v>
+      </c>
+      <c r="E7" s="6">
+        <v>119</v>
+      </c>
+      <c r="F7" s="6">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="8">
+        <v>45803</v>
+      </c>
+      <c r="B8" s="7">
+        <v>0.63402777777777775</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" s="6">
+        <v>53</v>
+      </c>
+      <c r="E8" s="6">
+        <v>115</v>
+      </c>
+      <c r="F8" s="6">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="8">
+        <v>45803</v>
+      </c>
+      <c r="B9" s="7">
+        <v>0.6430555555555556</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" s="6">
+        <v>57</v>
+      </c>
+      <c r="E9" s="6">
+        <v>118</v>
+      </c>
+      <c r="F9" s="6">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="5"/>
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
       <c r="D10" s="5"/>
       <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>